<commit_message>
add new labeled data
</commit_message>
<xml_diff>
--- a/data/grid_search_results/final_IncDec_roberta-large.xlsx
+++ b/data/grid_search_results/final_IncDec_roberta-large.xlsx
@@ -501,28 +501,28 @@
         <v>32</v>
       </c>
       <c r="D2" t="n">
-        <v>1.060579265866961</v>
+        <v>1.023045013436174</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5178571428571429</v>
+        <v>0.5221238938053098</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3533613445378152</v>
+        <v>0.4257391100668291</v>
       </c>
       <c r="G2" t="n">
-        <v>1.063753833162024</v>
+        <v>1.072624683380127</v>
       </c>
       <c r="H2" t="n">
-        <v>0.524822695035461</v>
+        <v>0.5140845070422535</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3612732970476661</v>
+        <v>0.4226176491197698</v>
       </c>
       <c r="J2" t="n">
-        <v>3.292092963059743</v>
+        <v>1.305260638395945</v>
       </c>
       <c r="K2" t="n">
-        <v>0.05862491528193156</v>
+        <v>0.008899195988972982</v>
       </c>
     </row>
     <row r="3">
@@ -536,28 +536,28 @@
         <v>32</v>
       </c>
       <c r="D3" t="n">
-        <v>1.744120836257935</v>
+        <v>1.295911005112977</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5982142857142857</v>
+        <v>0.7345132743362832</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6043796318179684</v>
+        <v>0.7340374916738034</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9879504873397502</v>
+        <v>1.630176624781649</v>
       </c>
       <c r="H3" t="n">
-        <v>0.6950354609929078</v>
+        <v>0.6408450704225352</v>
       </c>
       <c r="I3" t="n">
-        <v>0.6986947053436415</v>
+        <v>0.6391127734413041</v>
       </c>
       <c r="J3" t="n">
-        <v>10.69286740223567</v>
+        <v>4.597253056367238</v>
       </c>
       <c r="K3" t="n">
-        <v>0.05877751111984253</v>
+        <v>0.008896390597025553</v>
       </c>
     </row>
     <row r="4">
@@ -571,28 +571,28 @@
         <v>32</v>
       </c>
       <c r="D4" t="n">
-        <v>1.072283846991403</v>
+        <v>1.029749684629187</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4375</v>
+        <v>0.5486725663716814</v>
       </c>
       <c r="F4" t="n">
-        <v>0.420504173136646</v>
+        <v>0.4253720411650977</v>
       </c>
       <c r="G4" t="n">
-        <v>1.098024044476502</v>
+        <v>1.070262602517303</v>
       </c>
       <c r="H4" t="n">
-        <v>0.4326241134751773</v>
+        <v>0.5492957746478874</v>
       </c>
       <c r="I4" t="n">
-        <v>0.4172552814062248</v>
+        <v>0.4112402423173688</v>
       </c>
       <c r="J4" t="n">
-        <v>9.040680193901062</v>
+        <v>2.913654776414235</v>
       </c>
       <c r="K4" t="n">
-        <v>0.05864067475001018</v>
+        <v>0.008907381693522136</v>
       </c>
     </row>
     <row r="5">
@@ -606,28 +606,28 @@
         <v>32</v>
       </c>
       <c r="D5" t="n">
-        <v>1.373452050345285</v>
+        <v>1.42501640741804</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2589285714285715</v>
+        <v>0.1769911504424779</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1065096251266464</v>
+        <v>0.05323042118570763</v>
       </c>
       <c r="G5" t="n">
-        <v>1.373195922121089</v>
+        <v>1.426702490994628</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2695035460992908</v>
+        <v>0.2112676056338028</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1144260866119894</v>
+        <v>0.07369800196528006</v>
       </c>
       <c r="J5" t="n">
-        <v>3.294167315959931</v>
+        <v>1.303520202636719</v>
       </c>
       <c r="K5" t="n">
-        <v>0.05892614126205444</v>
+        <v>0.008923625946044922</v>
       </c>
     </row>
     <row r="6">
@@ -641,28 +641,28 @@
         <v>16</v>
       </c>
       <c r="D6" t="n">
-        <v>1.05270015341895</v>
+        <v>1.005135235005775</v>
       </c>
       <c r="E6" t="n">
-        <v>0.5178571428571429</v>
+        <v>0.5398230088495575</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3533613445378152</v>
+        <v>0.3784965924117586</v>
       </c>
       <c r="G6" t="n">
-        <v>1.054984089330579</v>
+        <v>1.024111437965447</v>
       </c>
       <c r="H6" t="n">
-        <v>0.524822695035461</v>
+        <v>0.5633802816901409</v>
       </c>
       <c r="I6" t="n">
-        <v>0.3612732970476661</v>
+        <v>0.4060398426595609</v>
       </c>
       <c r="J6" t="n">
-        <v>3.74632613658905</v>
+        <v>1.456115984916687</v>
       </c>
       <c r="K6" t="n">
-        <v>0.05835863749186198</v>
+        <v>0.00947255293528239</v>
       </c>
     </row>
     <row r="7">
@@ -676,28 +676,28 @@
         <v>16</v>
       </c>
       <c r="D7" t="n">
-        <v>1.568380236625671</v>
+        <v>1.377672099516587</v>
       </c>
       <c r="E7" t="n">
-        <v>0.5714285714285714</v>
+        <v>0.6814159292035398</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5879650297619047</v>
+        <v>0.6833582132636146</v>
       </c>
       <c r="G7" t="n">
-        <v>1.059349896214532</v>
+        <v>1.612589785750483</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6595744680851063</v>
+        <v>0.6056338028169014</v>
       </c>
       <c r="I7" t="n">
-        <v>0.6698175536719906</v>
+        <v>0.6110430842476368</v>
       </c>
       <c r="J7" t="n">
-        <v>7.970326189200083</v>
+        <v>4.829733387629191</v>
       </c>
       <c r="K7" t="n">
-        <v>0.05877012809117635</v>
+        <v>0.009604930877685547</v>
       </c>
     </row>
     <row r="8">
@@ -711,28 +711,28 @@
         <v>16</v>
       </c>
       <c r="D8" t="n">
-        <v>1.042240245001657</v>
+        <v>1.017042031330345</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5178571428571429</v>
+        <v>0.5309734513274337</v>
       </c>
       <c r="F8" t="n">
-        <v>0.4272224799010513</v>
+        <v>0.4040570049419606</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9977561852610703</v>
+        <v>1.016261535631099</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4680851063829787</v>
+        <v>0.5422535211267606</v>
       </c>
       <c r="I8" t="n">
-        <v>0.3497212518965456</v>
+        <v>0.4183607802767357</v>
       </c>
       <c r="J8" t="n">
-        <v>11.59211634000142</v>
+        <v>2.79915314912796</v>
       </c>
       <c r="K8" t="n">
-        <v>0.05885715087254842</v>
+        <v>0.009504803021748861</v>
       </c>
     </row>
     <row r="9">
@@ -746,28 +746,28 @@
         <v>16</v>
       </c>
       <c r="D9" t="n">
-        <v>1.371966166155679</v>
+        <v>1.421824205238207</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2589285714285715</v>
+        <v>0.1769911504424779</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1065096251266464</v>
+        <v>0.05323042118570763</v>
       </c>
       <c r="G9" t="n">
-        <v>1.37177844842275</v>
+        <v>1.423302601760542</v>
       </c>
       <c r="H9" t="n">
-        <v>0.2695035460992908</v>
+        <v>0.2112676056338028</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1144260866119894</v>
+        <v>0.07369800196528006</v>
       </c>
       <c r="J9" t="n">
-        <v>3.681834884484609</v>
+        <v>1.456860613822937</v>
       </c>
       <c r="K9" t="n">
-        <v>0.05881282091140747</v>
+        <v>0.009597273667653401</v>
       </c>
     </row>
     <row r="10">
@@ -781,28 +781,28 @@
         <v>8</v>
       </c>
       <c r="D10" t="n">
-        <v>1.061428189277649</v>
+        <v>0.9996407105859402</v>
       </c>
       <c r="E10" t="n">
-        <v>0.5178571428571429</v>
+        <v>0.5398230088495575</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3533613445378152</v>
+        <v>0.3784965924117586</v>
       </c>
       <c r="G10" t="n">
-        <v>1.060933347289444</v>
+        <v>1.009299950700411</v>
       </c>
       <c r="H10" t="n">
-        <v>0.524822695035461</v>
+        <v>0.5633802816901409</v>
       </c>
       <c r="I10" t="n">
-        <v>0.3612732970476661</v>
+        <v>0.4060398426595609</v>
       </c>
       <c r="J10" t="n">
-        <v>4.251017340024313</v>
+        <v>1.689779571692149</v>
       </c>
       <c r="K10" t="n">
-        <v>0.05533958673477173</v>
+        <v>0.01134317715962728</v>
       </c>
     </row>
     <row r="11">
@@ -816,28 +816,28 @@
         <v>8</v>
       </c>
       <c r="D11" t="n">
-        <v>1.144669747778348</v>
+        <v>1.421851219745369</v>
       </c>
       <c r="E11" t="n">
-        <v>0.5803571428571429</v>
+        <v>0.6902654867256637</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5799973835688121</v>
+        <v>0.6962865556251675</v>
       </c>
       <c r="G11" t="n">
-        <v>0.7213583711191272</v>
+        <v>1.829242202597605</v>
       </c>
       <c r="H11" t="n">
-        <v>0.6950354609929078</v>
+        <v>0.6267605633802817</v>
       </c>
       <c r="I11" t="n">
-        <v>0.6990480508405312</v>
+        <v>0.6281177976952624</v>
       </c>
       <c r="J11" t="n">
-        <v>7.877711363633474</v>
+        <v>4.752447664737701</v>
       </c>
       <c r="K11" t="n">
-        <v>0.05576324860254923</v>
+        <v>0.011222771803538</v>
       </c>
     </row>
     <row r="12">
@@ -851,28 +851,28 @@
         <v>8</v>
       </c>
       <c r="D12" t="n">
-        <v>0.9408132178442818</v>
+        <v>1.184708083625388</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5446428571428571</v>
+        <v>0.4513274336283186</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5510312268376784</v>
+        <v>0.3689773466047166</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8320484474195656</v>
+        <v>1.104946690545955</v>
       </c>
       <c r="H12" t="n">
-        <v>0.6879432624113475</v>
+        <v>0.5140845070422535</v>
       </c>
       <c r="I12" t="n">
-        <v>0.6918927020484575</v>
+        <v>0.4336163481158247</v>
       </c>
       <c r="J12" t="n">
-        <v>16.35734244187673</v>
+        <v>1.926286458969116</v>
       </c>
       <c r="K12" t="n">
-        <v>0.05585885842641194</v>
+        <v>0.01138545274734497</v>
       </c>
     </row>
     <row r="13">
@@ -886,28 +886,28 @@
         <v>8</v>
       </c>
       <c r="D13" t="n">
-        <v>1.368341952562332</v>
+        <v>1.415893305719426</v>
       </c>
       <c r="E13" t="n">
-        <v>0.2589285714285715</v>
+        <v>0.1769911504424779</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1065096251266464</v>
+        <v>0.05323042118570763</v>
       </c>
       <c r="G13" t="n">
-        <v>1.367886526364807</v>
+        <v>1.41728833863433</v>
       </c>
       <c r="H13" t="n">
-        <v>0.2695035460992908</v>
+        <v>0.2112676056338028</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1144260866119894</v>
+        <v>0.07369800196528006</v>
       </c>
       <c r="J13" t="n">
-        <v>4.264342749118805</v>
+        <v>1.693292045593262</v>
       </c>
       <c r="K13" t="n">
-        <v>0.05578232606252034</v>
+        <v>0.01124924818674723</v>
       </c>
     </row>
     <row r="14">
@@ -921,28 +921,28 @@
         <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>1.050895537648882</v>
+        <v>0.9987348238978766</v>
       </c>
       <c r="E14" t="n">
-        <v>0.5178571428571429</v>
+        <v>0.5398230088495575</v>
       </c>
       <c r="F14" t="n">
-        <v>0.3533613445378152</v>
+        <v>0.3784965924117586</v>
       </c>
       <c r="G14" t="n">
-        <v>1.050172849749842</v>
+        <v>0.9911463067565166</v>
       </c>
       <c r="H14" t="n">
-        <v>0.524822695035461</v>
+        <v>0.5633802816901409</v>
       </c>
       <c r="I14" t="n">
-        <v>0.3612732970476661</v>
+        <v>0.4060398426595609</v>
       </c>
       <c r="J14" t="n">
-        <v>5.194187339146932</v>
+        <v>2.182651408513387</v>
       </c>
       <c r="K14" t="n">
-        <v>0.05493222077687581</v>
+        <v>0.01289941072463989</v>
       </c>
     </row>
     <row r="15">
@@ -956,28 +956,28 @@
         <v>4</v>
       </c>
       <c r="D15" t="n">
-        <v>0.935151237196156</v>
+        <v>0.8315853381578902</v>
       </c>
       <c r="E15" t="n">
-        <v>0.5803571428571429</v>
+        <v>0.6371681415929203</v>
       </c>
       <c r="F15" t="n">
-        <v>0.5822229427007198</v>
+        <v>0.6268251882575817</v>
       </c>
       <c r="G15" t="n">
-        <v>0.7147630982048122</v>
+        <v>0.8583359441287081</v>
       </c>
       <c r="H15" t="n">
-        <v>0.7021276595744681</v>
+        <v>0.6056338028169014</v>
       </c>
       <c r="I15" t="n">
-        <v>0.7032604030239965</v>
+        <v>0.5942331849832726</v>
       </c>
       <c r="J15" t="n">
-        <v>10.88666886488597</v>
+        <v>3.052599859237671</v>
       </c>
       <c r="K15" t="n">
-        <v>0.05520039399464925</v>
+        <v>0.01304493347803752</v>
       </c>
     </row>
     <row r="16">
@@ -991,28 +991,28 @@
         <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9813140907457897</v>
+        <v>1.092340772130848</v>
       </c>
       <c r="E16" t="n">
-        <v>0.5178571428571429</v>
+        <v>0.4336283185840708</v>
       </c>
       <c r="F16" t="n">
-        <v>0.5071884600614439</v>
+        <v>0.401704261576732</v>
       </c>
       <c r="G16" t="n">
-        <v>0.8397391607575383</v>
+        <v>1.095511312216101</v>
       </c>
       <c r="H16" t="n">
-        <v>0.6453900709219859</v>
+        <v>0.4366197183098591</v>
       </c>
       <c r="I16" t="n">
-        <v>0.6517219946947246</v>
+        <v>0.3936253220598637</v>
       </c>
       <c r="J16" t="n">
-        <v>16.45407931407293</v>
+        <v>2.479187122980754</v>
       </c>
       <c r="K16" t="n">
-        <v>0.05522529284159342</v>
+        <v>0.01341335773468018</v>
       </c>
     </row>
     <row r="17">
@@ -1026,28 +1026,28 @@
         <v>4</v>
       </c>
       <c r="D17" t="n">
-        <v>1.365431932466371</v>
+        <v>1.410219321208718</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2589285714285715</v>
+        <v>0.1769911504424779</v>
       </c>
       <c r="F17" t="n">
-        <v>0.1065096251266464</v>
+        <v>0.05323042118570763</v>
       </c>
       <c r="G17" t="n">
-        <v>1.365326830258606</v>
+        <v>1.411538654649761</v>
       </c>
       <c r="H17" t="n">
-        <v>0.2695035460992908</v>
+        <v>0.2112676056338028</v>
       </c>
       <c r="I17" t="n">
-        <v>0.1144260866119894</v>
+        <v>0.07369800196528006</v>
       </c>
       <c r="J17" t="n">
-        <v>5.213240957260131</v>
+        <v>2.181176376342774</v>
       </c>
       <c r="K17" t="n">
-        <v>0.05523855288823445</v>
+        <v>0.01288429498672485</v>
       </c>
     </row>
     <row r="18">
@@ -1061,28 +1061,28 @@
         <v>32</v>
       </c>
       <c r="D18" t="n">
-        <v>1.032556312424796</v>
+        <v>0.9718156177385718</v>
       </c>
       <c r="E18" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F18" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G18" t="n">
-        <v>1.073411376763743</v>
+        <v>1.024264473310659</v>
       </c>
       <c r="H18" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J18" t="n">
-        <v>5.007330703735351</v>
+        <v>1.31103409131368</v>
       </c>
       <c r="K18" t="n">
-        <v>0.03520370324452718</v>
+        <v>0.0103053092956543</v>
       </c>
     </row>
     <row r="19">
@@ -1096,28 +1096,28 @@
         <v>32</v>
       </c>
       <c r="D19" t="n">
-        <v>1.002355141299111</v>
+        <v>0.9903513805001183</v>
       </c>
       <c r="E19" t="n">
-        <v>0.7410714285714286</v>
+        <v>0.6814159292035398</v>
       </c>
       <c r="F19" t="n">
-        <v>0.7488454997383569</v>
+        <v>0.6865558036544841</v>
       </c>
       <c r="G19" t="n">
-        <v>1.441361205797669</v>
+        <v>1.211526412359426</v>
       </c>
       <c r="H19" t="n">
-        <v>0.5602836879432624</v>
+        <v>0.5985915492957746</v>
       </c>
       <c r="I19" t="n">
-        <v>0.5562859627994111</v>
+        <v>0.6084580629019678</v>
       </c>
       <c r="J19" t="n">
-        <v>11.96486830711365</v>
+        <v>2.848132876555125</v>
       </c>
       <c r="K19" t="n">
-        <v>0.03525646924972534</v>
+        <v>0.01031804482142131</v>
       </c>
     </row>
     <row r="20">
@@ -1131,28 +1131,28 @@
         <v>32</v>
       </c>
       <c r="D20" t="n">
-        <v>1.030678749084473</v>
+        <v>0.996013215157838</v>
       </c>
       <c r="E20" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F20" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G20" t="n">
-        <v>1.076350603543275</v>
+        <v>1.021608213303794</v>
       </c>
       <c r="H20" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I20" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J20" t="n">
-        <v>5.03189834356308</v>
+        <v>1.306684462229411</v>
       </c>
       <c r="K20" t="n">
-        <v>0.03519728978474935</v>
+        <v>0.01030697027842204</v>
       </c>
     </row>
     <row r="21">
@@ -1166,28 +1166,28 @@
         <v>32</v>
       </c>
       <c r="D21" t="n">
-        <v>1.032291293144226</v>
+        <v>1.005559849528085</v>
       </c>
       <c r="E21" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F21" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G21" t="n">
-        <v>1.077202468899125</v>
+        <v>1.028784444634343</v>
       </c>
       <c r="H21" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J21" t="n">
-        <v>5.06427477200826</v>
+        <v>1.307420845826467</v>
       </c>
       <c r="K21" t="n">
-        <v>0.03513103326161703</v>
+        <v>0.01035090684890747</v>
       </c>
     </row>
     <row r="22">
@@ -1201,28 +1201,28 @@
         <v>16</v>
       </c>
       <c r="D22" t="n">
-        <v>1.037813365459442</v>
+        <v>0.9662084252433439</v>
       </c>
       <c r="E22" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F22" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G22" t="n">
-        <v>1.093059607431398</v>
+        <v>1.030403224515243</v>
       </c>
       <c r="H22" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I22" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J22" t="n">
-        <v>5.228685557842255</v>
+        <v>1.459053361415863</v>
       </c>
       <c r="K22" t="n">
-        <v>0.03668005069096883</v>
+        <v>0.01086403926213582</v>
       </c>
     </row>
     <row r="23">
@@ -1236,28 +1236,28 @@
         <v>16</v>
       </c>
       <c r="D23" t="n">
-        <v>0.843710890838078</v>
+        <v>1.513671566975361</v>
       </c>
       <c r="E23" t="n">
-        <v>0.6696428571428571</v>
+        <v>0.6814159292035398</v>
       </c>
       <c r="F23" t="n">
-        <v>0.6852681979800624</v>
+        <v>0.6732307528767707</v>
       </c>
       <c r="G23" t="n">
-        <v>1.156475572721333</v>
+        <v>1.965291987002735</v>
       </c>
       <c r="H23" t="n">
-        <v>0.5106382978723404</v>
+        <v>0.6126760563380281</v>
       </c>
       <c r="I23" t="n">
-        <v>0.5070685815366667</v>
+        <v>0.6022093010037627</v>
       </c>
       <c r="J23" t="n">
-        <v>13.4299676100413</v>
+        <v>3.749925116697947</v>
       </c>
       <c r="K23" t="n">
-        <v>0.03715427319208781</v>
+        <v>0.0109245777130127</v>
       </c>
     </row>
     <row r="24">
@@ -1271,28 +1271,28 @@
         <v>16</v>
       </c>
       <c r="D24" t="n">
-        <v>1.029704204627446</v>
+        <v>0.9932994378351532</v>
       </c>
       <c r="E24" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F24" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G24" t="n">
-        <v>1.077041332603346</v>
+        <v>1.019943853499184</v>
       </c>
       <c r="H24" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I24" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J24" t="n">
-        <v>5.289045774936676</v>
+        <v>1.45301274061203</v>
       </c>
       <c r="K24" t="n">
-        <v>0.03694870471954346</v>
+        <v>0.01079028050104777</v>
       </c>
     </row>
     <row r="25">
@@ -1306,28 +1306,28 @@
         <v>16</v>
       </c>
       <c r="D25" t="n">
-        <v>1.032241003853934</v>
+        <v>1.005227342116094</v>
       </c>
       <c r="E25" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F25" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G25" t="n">
-        <v>1.07728906472524</v>
+        <v>1.028611879953196</v>
       </c>
       <c r="H25" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I25" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J25" t="n">
-        <v>5.240798302491506</v>
+        <v>1.456234403451284</v>
       </c>
       <c r="K25" t="n">
-        <v>0.03718752066294352</v>
+        <v>0.01086873610814412</v>
       </c>
     </row>
     <row r="26">
@@ -1341,28 +1341,28 @@
         <v>8</v>
       </c>
       <c r="D26" t="n">
-        <v>1.026392553533827</v>
+        <v>0.9827633980101189</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F26" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G26" t="n">
-        <v>1.125198318603191</v>
+        <v>1.097513968675909</v>
       </c>
       <c r="H26" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I26" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J26" t="n">
-        <v>5.544094407558442</v>
+        <v>1.694418629010518</v>
       </c>
       <c r="K26" t="n">
-        <v>0.03714186350504557</v>
+        <v>0.01101398865381877</v>
       </c>
     </row>
     <row r="27">
@@ -1376,28 +1376,28 @@
         <v>8</v>
       </c>
       <c r="D27" t="n">
-        <v>1.194793341415269</v>
+        <v>0.8424739320721246</v>
       </c>
       <c r="E27" t="n">
-        <v>0.7857142857142857</v>
+        <v>0.672566371681416</v>
       </c>
       <c r="F27" t="n">
-        <v>0.7914971085885628</v>
+        <v>0.6713762428048141</v>
       </c>
       <c r="G27" t="n">
-        <v>2.083536376344397</v>
+        <v>0.8551392294991185</v>
       </c>
       <c r="H27" t="n">
-        <v>0.5460992907801419</v>
+        <v>0.6690140845070423</v>
       </c>
       <c r="I27" t="n">
-        <v>0.5483448037357018</v>
+        <v>0.6735516071255911</v>
       </c>
       <c r="J27" t="n">
-        <v>14.78063731193543</v>
+        <v>2.388712422053019</v>
       </c>
       <c r="K27" t="n">
-        <v>0.03762483994166056</v>
+        <v>0.01104469696680705</v>
       </c>
     </row>
     <row r="28">
@@ -1411,28 +1411,28 @@
         <v>8</v>
       </c>
       <c r="D28" t="n">
-        <v>1.029302188328334</v>
+        <v>0.9922291588994254</v>
       </c>
       <c r="E28" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F28" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G28" t="n">
-        <v>1.07686654557573</v>
+        <v>1.018744821279821</v>
       </c>
       <c r="H28" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I28" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J28" t="n">
-        <v>5.54915068546931</v>
+        <v>1.699626652399699</v>
       </c>
       <c r="K28" t="n">
-        <v>0.037623663743337</v>
+        <v>0.01123265822728475</v>
       </c>
     </row>
     <row r="29">
@@ -1446,28 +1446,28 @@
         <v>8</v>
       </c>
       <c r="D29" t="n">
-        <v>1.032127022743225</v>
+        <v>1.005137950973173</v>
       </c>
       <c r="E29" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F29" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G29" t="n">
-        <v>1.077231615993148</v>
+        <v>1.028453595201734</v>
       </c>
       <c r="H29" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I29" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J29" t="n">
-        <v>5.55388857126236</v>
+        <v>1.701192661126455</v>
       </c>
       <c r="K29" t="n">
-        <v>0.03759946425755819</v>
+        <v>0.01116495927174886</v>
       </c>
     </row>
     <row r="30">
@@ -1481,28 +1481,28 @@
         <v>4</v>
       </c>
       <c r="D30" t="n">
-        <v>1.016946247645787</v>
+        <v>1.049660644700042</v>
       </c>
       <c r="E30" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F30" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G30" t="n">
-        <v>1.070061277835927</v>
+        <v>1.181203961372375</v>
       </c>
       <c r="H30" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I30" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J30" t="n">
-        <v>6.271833113829294</v>
+        <v>2.185344076156616</v>
       </c>
       <c r="K30" t="n">
-        <v>0.04032114744186401</v>
+        <v>0.01363784869511922</v>
       </c>
     </row>
     <row r="31">
@@ -1516,28 +1516,28 @@
         <v>4</v>
       </c>
       <c r="D31" t="n">
-        <v>1.009677139776094</v>
+        <v>0.9643762259356743</v>
       </c>
       <c r="E31" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F31" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G31" t="n">
-        <v>1.07289933989234</v>
+        <v>1.009275630326338</v>
       </c>
       <c r="H31" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I31" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J31" t="n">
-        <v>6.265579481919606</v>
+        <v>2.189419651031494</v>
       </c>
       <c r="K31" t="n">
-        <v>0.04075365463892619</v>
+        <v>0.01399823824564616</v>
       </c>
     </row>
     <row r="32">
@@ -1551,28 +1551,28 @@
         <v>4</v>
       </c>
       <c r="D32" t="n">
-        <v>1.025549420288631</v>
+        <v>0.9836720956110321</v>
       </c>
       <c r="E32" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F32" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G32" t="n">
-        <v>1.074270978041574</v>
+        <v>1.012258754649632</v>
       </c>
       <c r="H32" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I32" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J32" t="n">
-        <v>6.270887227853139</v>
+        <v>2.184749984741211</v>
       </c>
       <c r="K32" t="n">
-        <v>0.04074434041976929</v>
+        <v>0.01331632534662882</v>
       </c>
     </row>
     <row r="33">
@@ -1586,28 +1586,28 @@
         <v>4</v>
       </c>
       <c r="D33" t="n">
-        <v>1.0318315412317</v>
+        <v>1.003718861436422</v>
       </c>
       <c r="E33" t="n">
-        <v>0.5357142857142857</v>
+        <v>0.6106194690265486</v>
       </c>
       <c r="F33" t="n">
-        <v>0.3737541528239203</v>
+        <v>0.4629971798113391</v>
       </c>
       <c r="G33" t="n">
-        <v>1.077008451975829</v>
+        <v>1.027417323958706</v>
       </c>
       <c r="H33" t="n">
-        <v>0.4539007092198581</v>
+        <v>0.5774647887323944</v>
       </c>
       <c r="I33" t="n">
-        <v>0.2834111745372773</v>
+        <v>0.4227867203219316</v>
       </c>
       <c r="J33" t="n">
-        <v>6.256456212202708</v>
+        <v>2.185254041353862</v>
       </c>
       <c r="K33" t="n">
-        <v>0.04066161314646403</v>
+        <v>0.01396548350652059</v>
       </c>
     </row>
     <row r="34">
@@ -1621,28 +1621,28 @@
         <v>32</v>
       </c>
       <c r="D34" t="n">
-        <v>1.15252115045275</v>
+        <v>0.9906992986138943</v>
       </c>
       <c r="E34" t="n">
-        <v>0.3571428571428572</v>
+        <v>0.5486725663716814</v>
       </c>
       <c r="F34" t="n">
-        <v>0.1879699248120301</v>
+        <v>0.3887737041719342</v>
       </c>
       <c r="G34" t="n">
-        <v>1.072332704320867</v>
+        <v>1.002913394444425</v>
       </c>
       <c r="H34" t="n">
-        <v>0.4609929078014184</v>
+        <v>0.5633802816901409</v>
       </c>
       <c r="I34" t="n">
-        <v>0.2909178544377883</v>
+        <v>0.4060398426595609</v>
       </c>
       <c r="J34" t="n">
-        <v>5.023207974433899</v>
+        <v>0.8609156131744384</v>
       </c>
       <c r="K34" t="n">
-        <v>0.03218005100886027</v>
+        <v>0.01611753304799398</v>
       </c>
     </row>
     <row r="35">
@@ -1656,28 +1656,28 @@
         <v>32</v>
       </c>
       <c r="D35" t="n">
-        <v>1.719980682645525</v>
+        <v>0.9908317084861012</v>
       </c>
       <c r="E35" t="n">
-        <v>0.6785714285714286</v>
+        <v>0.7256637168141593</v>
       </c>
       <c r="F35" t="n">
-        <v>0.6766261790537845</v>
+        <v>0.7273711124855726</v>
       </c>
       <c r="G35" t="n">
-        <v>1.544445784379404</v>
+        <v>1.448143490603272</v>
       </c>
       <c r="H35" t="n">
-        <v>0.6099290780141844</v>
+        <v>0.5985915492957746</v>
       </c>
       <c r="I35" t="n">
-        <v>0.6159916824847352</v>
+        <v>0.6057982195564227</v>
       </c>
       <c r="J35" t="n">
-        <v>16.16269923845927</v>
+        <v>2.287526734670003</v>
       </c>
       <c r="K35" t="n">
-        <v>0.03222471078236898</v>
+        <v>0.01619253953297933</v>
       </c>
     </row>
     <row r="36">
@@ -1691,28 +1691,28 @@
         <v>32</v>
       </c>
       <c r="D36" t="n">
-        <v>1.1132823910032</v>
+        <v>1.077982130303847</v>
       </c>
       <c r="E36" t="n">
-        <v>0.375</v>
+        <v>0.4867256637168141</v>
       </c>
       <c r="F36" t="n">
-        <v>0.2827720619928412</v>
+        <v>0.391740412979351</v>
       </c>
       <c r="G36" t="n">
-        <v>1.097381825988174</v>
+        <v>1.069624650646263</v>
       </c>
       <c r="H36" t="n">
-        <v>0.3687943262411347</v>
+        <v>0.5140845070422535</v>
       </c>
       <c r="I36" t="n">
-        <v>0.2957289978566575</v>
+        <v>0.4254665046114249</v>
       </c>
       <c r="J36" t="n">
-        <v>7.546485292911529</v>
+        <v>1.135869046052297</v>
       </c>
       <c r="K36" t="n">
-        <v>0.03217540184656779</v>
+        <v>0.0161981185277303</v>
       </c>
     </row>
     <row r="37">
@@ -1726,28 +1726,28 @@
         <v>32</v>
       </c>
       <c r="D37" t="n">
-        <v>1.128755024501256</v>
+        <v>1.175594707505893</v>
       </c>
       <c r="E37" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.1415929203539823</v>
       </c>
       <c r="F37" t="n">
-        <v>0.126984126984127</v>
+        <v>0.03512382520408863</v>
       </c>
       <c r="G37" t="n">
-        <v>1.145517914853198</v>
+        <v>1.163275989008622</v>
       </c>
       <c r="H37" t="n">
-        <v>0.2340425531914894</v>
+        <v>0.176056338028169</v>
       </c>
       <c r="I37" t="n">
-        <v>0.0887747615553925</v>
+        <v>0.0527114784515476</v>
       </c>
       <c r="J37" t="n">
-        <v>5.030187769730886</v>
+        <v>0.8687424739201863</v>
       </c>
       <c r="K37" t="n">
-        <v>0.0320196270942688</v>
+        <v>0.01617759068806966</v>
       </c>
     </row>
     <row r="38">
@@ -1761,28 +1761,28 @@
         <v>16</v>
       </c>
       <c r="D38" t="n">
-        <v>1.155394724437169</v>
+        <v>1.005367699977571</v>
       </c>
       <c r="E38" t="n">
-        <v>0.3571428571428572</v>
+        <v>0.5486725663716814</v>
       </c>
       <c r="F38" t="n">
-        <v>0.1879699248120301</v>
+        <v>0.3887737041719342</v>
       </c>
       <c r="G38" t="n">
-        <v>1.080576801130958</v>
+        <v>1.003742969371903</v>
       </c>
       <c r="H38" t="n">
-        <v>0.4609929078014184</v>
+        <v>0.5633802816901409</v>
       </c>
       <c r="I38" t="n">
-        <v>0.2909178544377883</v>
+        <v>0.4060398426595609</v>
       </c>
       <c r="J38" t="n">
-        <v>5.205470279852549</v>
+        <v>1.00324094692866</v>
       </c>
       <c r="K38" t="n">
-        <v>0.03429329792658488</v>
+        <v>0.01719506978988648</v>
       </c>
     </row>
     <row r="39">
@@ -1796,28 +1796,28 @@
         <v>16</v>
       </c>
       <c r="D39" t="n">
-        <v>1.646051040717534</v>
+        <v>0.9477968140117889</v>
       </c>
       <c r="E39" t="n">
-        <v>0.6160714285714286</v>
+        <v>0.7522123893805309</v>
       </c>
       <c r="F39" t="n">
-        <v>0.6079406887132963</v>
+        <v>0.756470222334809</v>
       </c>
       <c r="G39" t="n">
-        <v>1.519453489188607</v>
+        <v>1.798256068162515</v>
       </c>
       <c r="H39" t="n">
-        <v>0.6453900709219859</v>
+        <v>0.5422535211267606</v>
       </c>
       <c r="I39" t="n">
-        <v>0.6443747603170943</v>
+        <v>0.5507046608656266</v>
       </c>
       <c r="J39" t="n">
-        <v>13.75268706878026</v>
+        <v>2.207739698886871</v>
       </c>
       <c r="K39" t="n">
-        <v>0.03426278432210286</v>
+        <v>0.01724482377370199</v>
       </c>
     </row>
     <row r="40">
@@ -1831,28 +1831,28 @@
         <v>16</v>
       </c>
       <c r="D40" t="n">
-        <v>1.109502502850124</v>
+        <v>1.070557721948202</v>
       </c>
       <c r="E40" t="n">
-        <v>0.3571428571428572</v>
+        <v>0.4867256637168141</v>
       </c>
       <c r="F40" t="n">
-        <v>0.2707729245544371</v>
+        <v>0.3801168947763792</v>
       </c>
       <c r="G40" t="n">
-        <v>1.091619669122899</v>
+        <v>1.060878567292657</v>
       </c>
       <c r="H40" t="n">
-        <v>0.4113475177304964</v>
+        <v>0.4859154929577465</v>
       </c>
       <c r="I40" t="n">
-        <v>0.3054960386666002</v>
+        <v>0.3986400364669983</v>
       </c>
       <c r="J40" t="n">
-        <v>7.258255382378896</v>
+        <v>1.160275475184123</v>
       </c>
       <c r="K40" t="n">
-        <v>0.03426875273386638</v>
+        <v>0.01731892029444377</v>
       </c>
     </row>
     <row r="41">
@@ -1866,28 +1866,28 @@
         <v>16</v>
       </c>
       <c r="D41" t="n">
-        <v>1.128138252667018</v>
+        <v>1.173055317549579</v>
       </c>
       <c r="E41" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.1415929203539823</v>
       </c>
       <c r="F41" t="n">
-        <v>0.126984126984127</v>
+        <v>0.03512382520408863</v>
       </c>
       <c r="G41" t="n">
-        <v>1.144416408335909</v>
+        <v>1.160793974365987</v>
       </c>
       <c r="H41" t="n">
-        <v>0.2340425531914894</v>
+        <v>0.176056338028169</v>
       </c>
       <c r="I41" t="n">
-        <v>0.0887747615553925</v>
+        <v>0.0527114784515476</v>
       </c>
       <c r="J41" t="n">
-        <v>5.202223889032999</v>
+        <v>1.002774544556936</v>
       </c>
       <c r="K41" t="n">
-        <v>0.03417389392852783</v>
+        <v>0.01732954184214274</v>
       </c>
     </row>
     <row r="42">
@@ -1901,28 +1901,28 @@
         <v>8</v>
       </c>
       <c r="D42" t="n">
-        <v>1.125893541744777</v>
+        <v>1.019121847321502</v>
       </c>
       <c r="E42" t="n">
-        <v>0.3571428571428572</v>
+        <v>0.5486725663716814</v>
       </c>
       <c r="F42" t="n">
-        <v>0.1879699248120301</v>
+        <v>0.3887737041719342</v>
       </c>
       <c r="G42" t="n">
-        <v>1.068503492267419</v>
+        <v>1.007939639225812</v>
       </c>
       <c r="H42" t="n">
-        <v>0.4609929078014184</v>
+        <v>0.5633802816901409</v>
       </c>
       <c r="I42" t="n">
-        <v>0.2909178544377883</v>
+        <v>0.4060398426595609</v>
       </c>
       <c r="J42" t="n">
-        <v>5.54038458665212</v>
+        <v>1.233652472496033</v>
       </c>
       <c r="K42" t="n">
-        <v>0.03625754117965698</v>
+        <v>0.01765923500061035</v>
       </c>
     </row>
     <row r="43">
@@ -1936,28 +1936,28 @@
         <v>8</v>
       </c>
       <c r="D43" t="n">
-        <v>1.237752773932048</v>
+        <v>1.261883373940941</v>
       </c>
       <c r="E43" t="n">
-        <v>0.5535714285714286</v>
+        <v>0.7079646017699115</v>
       </c>
       <c r="F43" t="n">
-        <v>0.5503867201524053</v>
+        <v>0.7218695224659056</v>
       </c>
       <c r="G43" t="n">
-        <v>1.021804467583379</v>
+        <v>1.986534535465106</v>
       </c>
       <c r="H43" t="n">
-        <v>0.6028368794326241</v>
+        <v>0.5563380281690141</v>
       </c>
       <c r="I43" t="n">
-        <v>0.6060874704491725</v>
+        <v>0.5685866125367046</v>
       </c>
       <c r="J43" t="n">
-        <v>13.0883666396141</v>
+        <v>2.716978450616201</v>
       </c>
       <c r="K43" t="n">
-        <v>0.03655085166295369</v>
+        <v>0.01791167656580607</v>
       </c>
     </row>
     <row r="44">
@@ -1971,28 +1971,28 @@
         <v>8</v>
       </c>
       <c r="D44" t="n">
-        <v>1.110067444188254</v>
+        <v>1.039535701802347</v>
       </c>
       <c r="E44" t="n">
-        <v>0.3571428571428572</v>
+        <v>0.5486725663716814</v>
       </c>
       <c r="F44" t="n">
-        <v>0.2707828894269572</v>
+        <v>0.3887737041719342</v>
       </c>
       <c r="G44" t="n">
-        <v>1.093555547666888</v>
+        <v>1.040979147796899</v>
       </c>
       <c r="H44" t="n">
-        <v>0.425531914893617</v>
+        <v>0.5633802816901409</v>
       </c>
       <c r="I44" t="n">
-        <v>0.3282385507825717</v>
+        <v>0.4060398426595609</v>
       </c>
       <c r="J44" t="n">
-        <v>6.674691760540009</v>
+        <v>1.416583700974782</v>
       </c>
       <c r="K44" t="n">
-        <v>0.03685046037038167</v>
+        <v>0.01770507494608561</v>
       </c>
     </row>
     <row r="45">
@@ -2006,28 +2006,28 @@
         <v>8</v>
       </c>
       <c r="D45" t="n">
-        <v>1.127443083695003</v>
+        <v>1.170670490349289</v>
       </c>
       <c r="E45" t="n">
-        <v>0.2857142857142857</v>
+        <v>0.1415929203539823</v>
       </c>
       <c r="F45" t="n">
-        <v>0.126984126984127</v>
+        <v>0.03512382520408863</v>
       </c>
       <c r="G45" t="n">
-        <v>1.143164612722735</v>
+        <v>1.158610100477514</v>
       </c>
       <c r="H45" t="n">
-        <v>0.2340425531914894</v>
+        <v>0.176056338028169</v>
       </c>
       <c r="I45" t="n">
-        <v>0.0887747615553925</v>
+        <v>0.0527114784515476</v>
       </c>
       <c r="J45" t="n">
-        <v>5.538754240671794</v>
+        <v>1.229970252513886</v>
       </c>
       <c r="K45" t="n">
-        <v>0.03679828643798828</v>
+        <v>0.01791357199350993</v>
       </c>
     </row>
     <row r="46">
@@ -2041,28 +2041,28 @@
         <v>4</v>
       </c>
       <c r="D46" t="n">
-        <v>1.171877684337752</v>
+        <v>1.002730461348475</v>
       </c>
       <c r="E46" t="n">
-        <v>0.3571428571428572</v>
+        <v>0.5486725663716814</v>
       </c>
       <c r="F46" t="n">
-        <v>0.1879699248120301</v>
+        <v>0.3887737041719342</v>
       </c>
       <c r="G46" t="n">
-        <v>1.078467178852</v>
+        <v>0.9897418492276904</v>
       </c>
       <c r="H46" t="n">
-        <v>0.4609929078014184</v>
+        <v>0.5633802816901409</v>
       </c>
       <c r="I46" t="n">
-        <v>0.2909178544377883</v>
+        <v>0.4060398426595609</v>
       </c>
       <c r="J46" t="n">
-        <v>6.235312219460805</v>
+        <v>2.080215434233347</v>
       </c>
       <c r="K46" t="n">
-        <v>0.03940444787343343</v>
+        <v>0.01974633137385051</v>
       </c>
     </row>
     <row r="47">
@@ -2076,28 +2076,28 @@
         <v>4</v>
       </c>
       <c r="D47" t="n">
-        <v>1.22424603998661</v>
+        <v>0.80349921758196</v>
       </c>
       <c r="E47" t="n">
-        <v>0.6517857142857143</v>
+        <v>0.6902654867256637</v>
       </c>
       <c r="F47" t="n">
-        <v>0.6456136621315193</v>
+        <v>0.6844117178053464</v>
       </c>
       <c r="G47" t="n">
-        <v>1.020977357759121</v>
+        <v>0.8305758086728378</v>
       </c>
       <c r="H47" t="n">
-        <v>0.6524822695035462</v>
+        <v>0.6056338028169014</v>
       </c>
       <c r="I47" t="n">
-        <v>0.6477397407169111</v>
+        <v>0.5931428850883077</v>
       </c>
       <c r="J47" t="n">
-        <v>11.74168923298518</v>
+        <v>2.633215860525767</v>
       </c>
       <c r="K47" t="n">
-        <v>0.03994944890340169</v>
+        <v>0.01957984368006388</v>
       </c>
     </row>
     <row r="48">
@@ -2111,28 +2111,28 @@
         <v>4</v>
       </c>
       <c r="D48" t="n">
-        <v>1.113263028008597</v>
+        <v>1.063993112175865</v>
       </c>
       <c r="E48" t="n">
-        <v>0.2946428571428572</v>
+        <v>0.5486725663716814</v>
       </c>
       <c r="F48" t="n">
-        <v>0.2234667868846774</v>
+        <v>0.3910080358051063</v>
       </c>
       <c r="G48" t="n">
-        <v>1.099353056427435</v>
+        <v>1.056601433686807</v>
       </c>
       <c r="H48" t="n">
-        <v>0.2978723404255319</v>
+        <v>0.5633802816901409</v>
       </c>
       <c r="I48" t="n">
-        <v>0.2568035625927759</v>
+        <v>0.4097311139564661</v>
       </c>
       <c r="J48" t="n">
-        <v>6.254322306315104</v>
+        <v>2.074214140574137</v>
       </c>
       <c r="K48" t="n">
-        <v>0.03987835645675659</v>
+        <v>0.01982185443242391</v>
       </c>
     </row>
     <row r="49">
@@ -2146,28 +2146,28 @@
         <v>4</v>
       </c>
       <c r="D49" t="n">
-        <v>1.112382088388715</v>
+        <v>1.080428753278952</v>
       </c>
       <c r="E49" t="n">
-        <v>0.3214285714285715</v>
+        <v>0.4867256637168141</v>
       </c>
       <c r="F49" t="n">
-        <v>0.2507223113964687</v>
+        <v>0.3940211904813675</v>
       </c>
       <c r="G49" t="n">
-        <v>1.097618715137455</v>
+        <v>1.072570577473708</v>
       </c>
       <c r="H49" t="n">
-        <v>0.3475177304964539</v>
+        <v>0.4507042253521127</v>
       </c>
       <c r="I49" t="n">
-        <v>0.295731028189154</v>
+        <v>0.3717948717948718</v>
       </c>
       <c r="J49" t="n">
-        <v>16.09601115385691</v>
+        <v>4.479858863353729</v>
       </c>
       <c r="K49" t="n">
-        <v>0.0399374008178711</v>
+        <v>0.01982445319493612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>